<commit_message>
Fix mmseqs2 to not have the 100perc comparison
</commit_message>
<xml_diff>
--- a/results/tables/Counted_correctness.xlsx
+++ b/results/tables/Counted_correctness.xlsx
@@ -451,7 +451,7 @@
         <v>99</v>
       </c>
       <c r="K2">
-        <v>13.13131313131313</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="3">
@@ -587,7 +587,7 @@
         <v>99</v>
       </c>
       <c r="K6">
-        <v>7.07070707070707</v>
+        <v>7.07</v>
       </c>
     </row>
     <row r="7">
@@ -630,7 +630,7 @@
         <v>99</v>
       </c>
       <c r="K7">
-        <v>6.060606060606061</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="8">
@@ -673,7 +673,7 @@
         <v>99</v>
       </c>
       <c r="K8">
-        <v>14.14141414141414</v>
+        <v>14.14</v>
       </c>
     </row>
     <row r="9">
@@ -716,7 +716,7 @@
         <v>99</v>
       </c>
       <c r="K9">
-        <v>59.59595959595959</v>
+        <v>59.6</v>
       </c>
     </row>
     <row r="10">
@@ -756,7 +756,7 @@
         <v>99</v>
       </c>
       <c r="K10">
-        <v>27.27272727272727</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="11">
@@ -892,7 +892,7 @@
         <v>99</v>
       </c>
       <c r="K14">
-        <v>7.07070707070707</v>
+        <v>7.07</v>
       </c>
     </row>
     <row r="15">
@@ -966,7 +966,7 @@
         <v>99</v>
       </c>
       <c r="K16">
-        <v>14.14141414141414</v>
+        <v>14.14</v>
       </c>
     </row>
     <row r="17">
@@ -1009,7 +1009,7 @@
         <v>99</v>
       </c>
       <c r="K17">
-        <v>51.51515151515152</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="18">
@@ -1049,7 +1049,7 @@
         <v>99</v>
       </c>
       <c r="K18">
-        <v>4.040404040404041</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="19">
@@ -1092,7 +1092,7 @@
         <v>99</v>
       </c>
       <c r="K19">
-        <v>3.03030303030303</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="20">
@@ -1166,7 +1166,7 @@
         <v>99</v>
       </c>
       <c r="K21">
-        <v>2.02020202020202</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="22">
@@ -1209,7 +1209,7 @@
         <v>99</v>
       </c>
       <c r="K22">
-        <v>16.16161616161616</v>
+        <v>16.16</v>
       </c>
     </row>
     <row r="23">
@@ -1252,7 +1252,7 @@
         <v>99</v>
       </c>
       <c r="K23">
-        <v>6.060606060606061</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="24">
@@ -1295,7 +1295,7 @@
         <v>99</v>
       </c>
       <c r="K24">
-        <v>20.2020202020202</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="25">
@@ -1338,7 +1338,7 @@
         <v>99</v>
       </c>
       <c r="K25">
-        <v>48.48484848484848</v>
+        <v>48.48</v>
       </c>
     </row>
     <row r="26">
@@ -1378,7 +1378,7 @@
         <v>99</v>
       </c>
       <c r="K26">
-        <v>11.11111111111111</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="27">
@@ -1452,7 +1452,7 @@
         <v>99</v>
       </c>
       <c r="K28">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="29">
@@ -1526,7 +1526,7 @@
         <v>99</v>
       </c>
       <c r="K30">
-        <v>16.16161616161616</v>
+        <v>16.16</v>
       </c>
     </row>
     <row r="31">
@@ -1569,7 +1569,7 @@
         <v>99</v>
       </c>
       <c r="K31">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="32">
@@ -1612,7 +1612,7 @@
         <v>99</v>
       </c>
       <c r="K32">
-        <v>18.18181818181818</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="33">
@@ -1655,7 +1655,7 @@
         <v>99</v>
       </c>
       <c r="K33">
-        <v>48.48484848484848</v>
+        <v>48.48</v>
       </c>
     </row>
     <row r="34">
@@ -1769,7 +1769,7 @@
         <v>99</v>
       </c>
       <c r="K36">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="37">
@@ -1812,7 +1812,7 @@
         <v>99</v>
       </c>
       <c r="K37">
-        <v>6.060606060606061</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="38">
@@ -1855,7 +1855,7 @@
         <v>99</v>
       </c>
       <c r="K38">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="39">
@@ -1898,7 +1898,7 @@
         <v>99</v>
       </c>
       <c r="K39">
-        <v>8.080808080808081</v>
+        <v>8.08</v>
       </c>
     </row>
     <row r="40">
@@ -1941,7 +1941,7 @@
         <v>99</v>
       </c>
       <c r="K40">
-        <v>20.2020202020202</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="41">
@@ -1984,7 +1984,7 @@
         <v>99</v>
       </c>
       <c r="K41">
-        <v>54.54545454545454</v>
+        <v>54.55</v>
       </c>
     </row>
     <row r="42">
@@ -2027,7 +2027,7 @@
         <v>99</v>
       </c>
       <c r="K42">
-        <v>3.03030303030303</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="43">
@@ -2172,7 +2172,7 @@
         <v>99</v>
       </c>
       <c r="K46">
-        <v>3.03030303030303</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="47">
@@ -2215,7 +2215,7 @@
         <v>99</v>
       </c>
       <c r="K47">
-        <v>9.090909090909092</v>
+        <v>9.09</v>
       </c>
     </row>
     <row r="48">
@@ -2258,7 +2258,7 @@
         <v>99</v>
       </c>
       <c r="K48">
-        <v>12.12121212121212</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="49">
@@ -2301,7 +2301,7 @@
         <v>99</v>
       </c>
       <c r="K49">
-        <v>20.2020202020202</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="50">
@@ -2344,7 +2344,7 @@
         <v>99</v>
       </c>
       <c r="K50">
-        <v>52.52525252525253</v>
+        <v>52.53</v>
       </c>
     </row>
     <row r="51">
@@ -2387,7 +2387,7 @@
         <v>99</v>
       </c>
       <c r="K51">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="52">
@@ -2532,7 +2532,7 @@
         <v>99</v>
       </c>
       <c r="K55">
-        <v>2.02020202020202</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="56">
@@ -2575,7 +2575,7 @@
         <v>99</v>
       </c>
       <c r="K56">
-        <v>15.15151515151515</v>
+        <v>15.15</v>
       </c>
     </row>
     <row r="57">
@@ -2618,7 +2618,7 @@
         <v>99</v>
       </c>
       <c r="K57">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="58">
@@ -2661,7 +2661,7 @@
         <v>99</v>
       </c>
       <c r="K58">
-        <v>25.25252525252525</v>
+        <v>25.25</v>
       </c>
     </row>
     <row r="59">
@@ -2704,7 +2704,7 @@
         <v>99</v>
       </c>
       <c r="K59">
-        <v>51.51515151515152</v>
+        <v>51.52</v>
       </c>
     </row>
     <row r="60">
@@ -2747,7 +2747,7 @@
         <v>99</v>
       </c>
       <c r="K60">
-        <v>3.03030303030303</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="61">
@@ -2892,7 +2892,7 @@
         <v>99</v>
       </c>
       <c r="K64">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="65">
@@ -2935,7 +2935,7 @@
         <v>99</v>
       </c>
       <c r="K65">
-        <v>13.13131313131313</v>
+        <v>13.13</v>
       </c>
     </row>
     <row r="66">
@@ -2978,7 +2978,7 @@
         <v>99</v>
       </c>
       <c r="K66">
-        <v>12.12121212121212</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="67">
@@ -3021,7 +3021,7 @@
         <v>99</v>
       </c>
       <c r="K67">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="68">
@@ -3064,7 +3064,7 @@
         <v>99</v>
       </c>
       <c r="K68">
-        <v>48.48484848484848</v>
+        <v>48.48</v>
       </c>
     </row>
     <row r="69">
@@ -3107,7 +3107,7 @@
         <v>99</v>
       </c>
       <c r="K69">
-        <v>2.02020202020202</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="70">
@@ -3252,7 +3252,7 @@
         <v>99</v>
       </c>
       <c r="K73">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="74">
@@ -3295,7 +3295,7 @@
         <v>99</v>
       </c>
       <c r="K74">
-        <v>18.18181818181818</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="75">
@@ -3338,7 +3338,7 @@
         <v>99</v>
       </c>
       <c r="K75">
-        <v>4.040404040404041</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="76">
@@ -3381,7 +3381,7 @@
         <v>99</v>
       </c>
       <c r="K76">
-        <v>27.27272727272727</v>
+        <v>27.27</v>
       </c>
     </row>
     <row r="77">
@@ -3424,7 +3424,7 @@
         <v>99</v>
       </c>
       <c r="K77">
-        <v>47.47474747474747</v>
+        <v>47.47</v>
       </c>
     </row>
     <row r="78">
@@ -3467,7 +3467,7 @@
         <v>99</v>
       </c>
       <c r="K78">
-        <v>3.03030303030303</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="79">
@@ -3643,7 +3643,7 @@
         <v>99</v>
       </c>
       <c r="K83">
-        <v>17.17171717171717</v>
+        <v>17.17</v>
       </c>
     </row>
     <row r="84">
@@ -3686,7 +3686,7 @@
         <v>99</v>
       </c>
       <c r="K84">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="85">
@@ -3729,7 +3729,7 @@
         <v>99</v>
       </c>
       <c r="K85">
-        <v>24.24242424242424</v>
+        <v>24.24</v>
       </c>
     </row>
     <row r="86">
@@ -3772,7 +3772,7 @@
         <v>99</v>
       </c>
       <c r="K86">
-        <v>45.45454545454545</v>
+        <v>45.45</v>
       </c>
     </row>
     <row r="87">
@@ -3815,7 +3815,7 @@
         <v>99</v>
       </c>
       <c r="K87">
-        <v>19.19191919191919</v>
+        <v>19.19</v>
       </c>
     </row>
     <row r="88">
@@ -3929,7 +3929,7 @@
         <v>99</v>
       </c>
       <c r="K90">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="91">
@@ -4003,7 +4003,7 @@
         <v>99</v>
       </c>
       <c r="K92">
-        <v>6.060606060606061</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="93">
@@ -4077,7 +4077,7 @@
         <v>99</v>
       </c>
       <c r="K94">
-        <v>14.14141414141414</v>
+        <v>14.14</v>
       </c>
     </row>
     <row r="95">
@@ -4120,7 +4120,7 @@
         <v>99</v>
       </c>
       <c r="K95">
-        <v>59.59595959595959</v>
+        <v>59.6</v>
       </c>
     </row>
     <row r="96">
@@ -4163,7 +4163,7 @@
         <v>99</v>
       </c>
       <c r="K96">
-        <v>20.2020202020202</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="97">
@@ -4339,7 +4339,7 @@
         <v>99</v>
       </c>
       <c r="K101">
-        <v>4.040404040404041</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="102">
@@ -4413,7 +4413,7 @@
         <v>99</v>
       </c>
       <c r="K103">
-        <v>15.15151515151515</v>
+        <v>15.15</v>
       </c>
     </row>
     <row r="104">
@@ -4456,7 +4456,7 @@
         <v>99</v>
       </c>
       <c r="K104">
-        <v>60.60606060606061</v>
+        <v>60.61</v>
       </c>
     </row>
     <row r="105">
@@ -4499,7 +4499,7 @@
         <v>99</v>
       </c>
       <c r="K105">
-        <v>38.38383838383838</v>
+        <v>38.38</v>
       </c>
     </row>
     <row r="106">
@@ -4644,7 +4644,7 @@
         <v>99</v>
       </c>
       <c r="K109">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="110">
@@ -4718,7 +4718,7 @@
         <v>99</v>
       </c>
       <c r="K111">
-        <v>15.15151515151515</v>
+        <v>15.15</v>
       </c>
     </row>
     <row r="112">
@@ -4792,7 +4792,7 @@
         <v>99</v>
       </c>
       <c r="K113">
-        <v>41.41414141414141</v>
+        <v>41.41</v>
       </c>
     </row>
     <row r="114">
@@ -4835,7 +4835,7 @@
         <v>99</v>
       </c>
       <c r="K114">
-        <v>35.35353535353536</v>
+        <v>35.35</v>
       </c>
     </row>
     <row r="115">
@@ -4980,7 +4980,7 @@
         <v>99</v>
       </c>
       <c r="K118">
-        <v>4.040404040404041</v>
+        <v>4.04</v>
       </c>
     </row>
     <row r="119">
@@ -5054,7 +5054,7 @@
         <v>99</v>
       </c>
       <c r="K120">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="121">
@@ -5128,7 +5128,7 @@
         <v>99</v>
       </c>
       <c r="K122">
-        <v>50.50505050505051</v>
+        <v>50.51</v>
       </c>
     </row>
     <row r="123">
@@ -5171,7 +5171,7 @@
         <v>99</v>
       </c>
       <c r="K123">
-        <v>38.38383838383838</v>
+        <v>38.38</v>
       </c>
     </row>
     <row r="124">
@@ -5316,7 +5316,7 @@
         <v>99</v>
       </c>
       <c r="K127">
-        <v>1.01010101010101</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="128">
@@ -5390,7 +5390,7 @@
         <v>99</v>
       </c>
       <c r="K129">
-        <v>18.18181818181818</v>
+        <v>18.18</v>
       </c>
     </row>
     <row r="130">
@@ -5464,7 +5464,7 @@
         <v>99</v>
       </c>
       <c r="K131">
-        <v>42.42424242424242</v>
+        <v>42.42</v>
       </c>
     </row>
     <row r="132">
@@ -5507,7 +5507,7 @@
         <v>99</v>
       </c>
       <c r="K132">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="133">
@@ -5652,7 +5652,7 @@
         <v>99</v>
       </c>
       <c r="K136">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="137">
@@ -5726,7 +5726,7 @@
         <v>99</v>
       </c>
       <c r="K138">
-        <v>7.07070707070707</v>
+        <v>7.07</v>
       </c>
     </row>
     <row r="139">
@@ -5800,7 +5800,7 @@
         <v>99</v>
       </c>
       <c r="K140">
-        <v>54.54545454545454</v>
+        <v>54.55</v>
       </c>
     </row>
     <row r="141">
@@ -5840,7 +5840,7 @@
         <v>99</v>
       </c>
       <c r="K141">
-        <v>48.48484848484848</v>
+        <v>48.48</v>
       </c>
     </row>
     <row r="142">
@@ -5945,7 +5945,7 @@
         <v>99</v>
       </c>
       <c r="K144">
-        <v>6.060606060606061</v>
+        <v>6.06</v>
       </c>
     </row>
     <row r="145">
@@ -6019,7 +6019,7 @@
         <v>99</v>
       </c>
       <c r="K146">
-        <v>16.16161616161616</v>
+        <v>16.16</v>
       </c>
     </row>
     <row r="147">
@@ -6093,7 +6093,7 @@
         <v>99</v>
       </c>
       <c r="K148">
-        <v>29.29292929292929</v>
+        <v>29.29</v>
       </c>
     </row>
     <row r="149">
@@ -6133,7 +6133,7 @@
         <v>99</v>
       </c>
       <c r="K149">
-        <v>42.42424242424242</v>
+        <v>42.42</v>
       </c>
     </row>
     <row r="150">
@@ -6238,7 +6238,7 @@
         <v>99</v>
       </c>
       <c r="K152">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="153">
@@ -6312,7 +6312,7 @@
         <v>99</v>
       </c>
       <c r="K154">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="155">
@@ -6386,7 +6386,7 @@
         <v>99</v>
       </c>
       <c r="K156">
-        <v>42.42424242424242</v>
+        <v>42.42</v>
       </c>
     </row>
     <row r="157">
@@ -6429,7 +6429,7 @@
         <v>99</v>
       </c>
       <c r="K157">
-        <v>63.63636363636363</v>
+        <v>63.64</v>
       </c>
     </row>
     <row r="158">
@@ -6574,7 +6574,7 @@
         <v>99</v>
       </c>
       <c r="K161">
-        <v>2.02020202020202</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="162">
@@ -6648,7 +6648,7 @@
         <v>99</v>
       </c>
       <c r="K163">
-        <v>12.12121212121212</v>
+        <v>12.12</v>
       </c>
     </row>
     <row r="164">
@@ -6722,7 +6722,7 @@
         <v>99</v>
       </c>
       <c r="K165">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="166">
@@ -6762,7 +6762,7 @@
         <v>99</v>
       </c>
       <c r="K166">
-        <v>44.44444444444444</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="167">
@@ -6867,7 +6867,7 @@
         <v>99</v>
       </c>
       <c r="K169">
-        <v>5.05050505050505</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="170">
@@ -6941,7 +6941,7 @@
         <v>99</v>
       </c>
       <c r="K171">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="172">
@@ -7015,7 +7015,7 @@
         <v>99</v>
       </c>
       <c r="K173">
-        <v>40.4040404040404</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="174">
@@ -7055,7 +7055,7 @@
         <v>99</v>
       </c>
       <c r="K174">
-        <v>44.44444444444444</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="175">
@@ -7160,7 +7160,7 @@
         <v>99</v>
       </c>
       <c r="K177">
-        <v>2.02020202020202</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="178">
@@ -7234,7 +7234,7 @@
         <v>99</v>
       </c>
       <c r="K179">
-        <v>10.1010101010101</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="180">
@@ -7308,7 +7308,7 @@
         <v>99</v>
       </c>
       <c r="K181">
-        <v>43.43434343434344</v>
+        <v>43.43</v>
       </c>
     </row>
     <row r="182">
@@ -7348,7 +7348,7 @@
         <v>24</v>
       </c>
       <c r="K182">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="183">
@@ -7484,7 +7484,7 @@
         <v>24</v>
       </c>
       <c r="K186">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="187">
@@ -7527,7 +7527,7 @@
         <v>24</v>
       </c>
       <c r="K187">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="188">
@@ -7613,7 +7613,7 @@
         <v>24</v>
       </c>
       <c r="K189">
-        <v>58.33333333333334</v>
+        <v>58.33</v>
       </c>
     </row>
     <row r="190">
@@ -7653,7 +7653,7 @@
         <v>27</v>
       </c>
       <c r="K190">
-        <v>51.85185185185185</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="191">
@@ -7789,7 +7789,7 @@
         <v>27</v>
       </c>
       <c r="K194">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="195">
@@ -7832,7 +7832,7 @@
         <v>27</v>
       </c>
       <c r="K195">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="196">
@@ -7875,7 +7875,7 @@
         <v>27</v>
       </c>
       <c r="K196">
-        <v>7.407407407407407</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="197">
@@ -7918,7 +7918,7 @@
         <v>27</v>
       </c>
       <c r="K197">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="198">
@@ -7958,7 +7958,7 @@
         <v>24</v>
       </c>
       <c r="K198">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="199">
@@ -8137,7 +8137,7 @@
         <v>24</v>
       </c>
       <c r="K203">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="204">
@@ -8263,7 +8263,7 @@
         <v>27</v>
       </c>
       <c r="K206">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="207">
@@ -8368,7 +8368,7 @@
         <v>27</v>
       </c>
       <c r="K209">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="210">
@@ -8411,7 +8411,7 @@
         <v>27</v>
       </c>
       <c r="K210">
-        <v>11.11111111111111</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="211">
@@ -8454,7 +8454,7 @@
         <v>27</v>
       </c>
       <c r="K211">
-        <v>7.407407407407407</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="212">
@@ -8497,7 +8497,7 @@
         <v>27</v>
       </c>
       <c r="K212">
-        <v>11.11111111111111</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="213">
@@ -8540,7 +8540,7 @@
         <v>27</v>
       </c>
       <c r="K213">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="214">
@@ -8716,7 +8716,7 @@
         <v>24</v>
       </c>
       <c r="K218">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="219">
@@ -8759,7 +8759,7 @@
         <v>24</v>
       </c>
       <c r="K219">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="220">
@@ -8802,7 +8802,7 @@
         <v>24</v>
       </c>
       <c r="K220">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="221">
@@ -8845,7 +8845,7 @@
         <v>24</v>
       </c>
       <c r="K221">
-        <v>66.66666666666666</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="222">
@@ -8990,7 +8990,7 @@
         <v>27</v>
       </c>
       <c r="K225">
-        <v>14.81481481481481</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="226">
@@ -9033,7 +9033,7 @@
         <v>27</v>
       </c>
       <c r="K226">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="227">
@@ -9076,7 +9076,7 @@
         <v>27</v>
       </c>
       <c r="K227">
-        <v>29.62962962962963</v>
+        <v>29.63</v>
       </c>
     </row>
     <row r="228">
@@ -9119,7 +9119,7 @@
         <v>27</v>
       </c>
       <c r="K228">
-        <v>14.81481481481481</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="229">
@@ -9162,7 +9162,7 @@
         <v>27</v>
       </c>
       <c r="K229">
-        <v>37.03703703703704</v>
+        <v>37.04</v>
       </c>
     </row>
     <row r="230">
@@ -9338,7 +9338,7 @@
         <v>24</v>
       </c>
       <c r="K234">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="235">
@@ -9381,7 +9381,7 @@
         <v>24</v>
       </c>
       <c r="K235">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="236">
@@ -9424,7 +9424,7 @@
         <v>24</v>
       </c>
       <c r="K236">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="237">
@@ -9467,7 +9467,7 @@
         <v>24</v>
       </c>
       <c r="K237">
-        <v>54.16666666666666</v>
+        <v>54.17</v>
       </c>
     </row>
     <row r="238">
@@ -9510,7 +9510,7 @@
         <v>27</v>
       </c>
       <c r="K238">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="239">
@@ -9655,7 +9655,7 @@
         <v>27</v>
       </c>
       <c r="K242">
-        <v>11.11111111111111</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="243">
@@ -9698,7 +9698,7 @@
         <v>27</v>
       </c>
       <c r="K243">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="244">
@@ -9741,7 +9741,7 @@
         <v>27</v>
       </c>
       <c r="K244">
-        <v>14.81481481481481</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="245">
@@ -9784,7 +9784,7 @@
         <v>27</v>
       </c>
       <c r="K245">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="246">
@@ -9827,7 +9827,7 @@
         <v>27</v>
       </c>
       <c r="K246">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="247">
@@ -10003,7 +10003,7 @@
         <v>24</v>
       </c>
       <c r="K251">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="252">
@@ -10077,7 +10077,7 @@
         <v>24</v>
       </c>
       <c r="K253">
-        <v>54.16666666666666</v>
+        <v>54.17</v>
       </c>
     </row>
     <row r="254">
@@ -10163,7 +10163,7 @@
         <v>27</v>
       </c>
       <c r="K255">
-        <v>14.81481481481481</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="256">
@@ -10308,7 +10308,7 @@
         <v>27</v>
       </c>
       <c r="K259">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="260">
@@ -10351,7 +10351,7 @@
         <v>27</v>
       </c>
       <c r="K260">
-        <v>14.81481481481481</v>
+        <v>14.81</v>
       </c>
     </row>
     <row r="261">
@@ -10394,7 +10394,7 @@
         <v>27</v>
       </c>
       <c r="K261">
-        <v>11.11111111111111</v>
+        <v>11.11</v>
       </c>
     </row>
     <row r="262">
@@ -10437,7 +10437,7 @@
         <v>27</v>
       </c>
       <c r="K262">
-        <v>25.92592592592592</v>
+        <v>25.93</v>
       </c>
     </row>
     <row r="263">
@@ -10480,7 +10480,7 @@
         <v>27</v>
       </c>
       <c r="K263">
-        <v>29.62962962962963</v>
+        <v>29.63</v>
       </c>
     </row>
     <row r="264">
@@ -10523,7 +10523,7 @@
         <v>24</v>
       </c>
       <c r="K264">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="265">
@@ -10761,7 +10761,7 @@
         <v>24</v>
       </c>
       <c r="K271">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="272">
@@ -10804,7 +10804,7 @@
         <v>24</v>
       </c>
       <c r="K272">
-        <v>66.66666666666666</v>
+        <v>66.67</v>
       </c>
     </row>
     <row r="273">
@@ -10847,7 +10847,7 @@
         <v>27</v>
       </c>
       <c r="K273">
-        <v>55.55555555555556</v>
+        <v>55.56</v>
       </c>
     </row>
     <row r="274">
@@ -11085,7 +11085,7 @@
         <v>27</v>
       </c>
       <c r="K280">
-        <v>7.407407407407407</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="281">
@@ -11128,7 +11128,7 @@
         <v>27</v>
       </c>
       <c r="K281">
-        <v>37.03703703703704</v>
+        <v>37.04</v>
       </c>
     </row>
     <row r="282">
@@ -11347,7 +11347,7 @@
         <v>24</v>
       </c>
       <c r="K287">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="288">
@@ -11390,7 +11390,7 @@
         <v>24</v>
       </c>
       <c r="K288">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="289">
@@ -11507,7 +11507,7 @@
         <v>27</v>
       </c>
       <c r="K291">
-        <v>44.44444444444444</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="292">
@@ -11652,7 +11652,7 @@
         <v>27</v>
       </c>
       <c r="K295">
-        <v>7.407407407407407</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="296">
@@ -11695,7 +11695,7 @@
         <v>27</v>
       </c>
       <c r="K296">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="297">
@@ -11738,7 +11738,7 @@
         <v>27</v>
       </c>
       <c r="K297">
-        <v>18.51851851851852</v>
+        <v>18.52</v>
       </c>
     </row>
     <row r="298">
@@ -11812,7 +11812,7 @@
         <v>27</v>
       </c>
       <c r="K299">
-        <v>25.92592592592592</v>
+        <v>25.93</v>
       </c>
     </row>
     <row r="300">
@@ -11855,7 +11855,7 @@
         <v>24</v>
       </c>
       <c r="K300">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="301">
@@ -12062,7 +12062,7 @@
         <v>24</v>
       </c>
       <c r="K306">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="307">
@@ -12179,7 +12179,7 @@
         <v>27</v>
       </c>
       <c r="K309">
-        <v>62.96296296296296</v>
+        <v>62.96</v>
       </c>
     </row>
     <row r="310">
@@ -12386,7 +12386,7 @@
         <v>27</v>
       </c>
       <c r="K315">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="316">
@@ -12460,7 +12460,7 @@
         <v>27</v>
       </c>
       <c r="K317">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="318">
@@ -12667,7 +12667,7 @@
         <v>24</v>
       </c>
       <c r="K323">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="324">
@@ -12741,7 +12741,7 @@
         <v>24</v>
       </c>
       <c r="K325">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="326">
@@ -12781,7 +12781,7 @@
         <v>27</v>
       </c>
       <c r="K326">
-        <v>51.85185185185185</v>
+        <v>51.85</v>
       </c>
     </row>
     <row r="327">
@@ -12917,7 +12917,7 @@
         <v>27</v>
       </c>
       <c r="K330">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="331">
@@ -12960,7 +12960,7 @@
         <v>27</v>
       </c>
       <c r="K331">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="332">
@@ -13034,7 +13034,7 @@
         <v>27</v>
       </c>
       <c r="K333">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="334">
@@ -13077,7 +13077,7 @@
         <v>24</v>
       </c>
       <c r="K334">
-        <v>29.16666666666667</v>
+        <v>29.17</v>
       </c>
     </row>
     <row r="335">
@@ -13253,7 +13253,7 @@
         <v>24</v>
       </c>
       <c r="K339">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="340">
@@ -13296,7 +13296,7 @@
         <v>24</v>
       </c>
       <c r="K340">
-        <v>8.333333333333332</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="341">
@@ -13370,7 +13370,7 @@
         <v>24</v>
       </c>
       <c r="K342">
-        <v>58.33333333333334</v>
+        <v>58.33</v>
       </c>
     </row>
     <row r="343">
@@ -13410,7 +13410,7 @@
         <v>24</v>
       </c>
       <c r="K343">
-        <v>45.83333333333333</v>
+        <v>45.83</v>
       </c>
     </row>
     <row r="344">
@@ -13546,7 +13546,7 @@
         <v>24</v>
       </c>
       <c r="K347">
-        <v>4.166666666666666</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="348">
@@ -13589,7 +13589,7 @@
         <v>24</v>
       </c>
       <c r="K348">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="349">
@@ -13663,7 +13663,7 @@
         <v>24</v>
       </c>
       <c r="K350">
-        <v>33.33333333333333</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="351">
@@ -13703,7 +13703,7 @@
         <v>27</v>
       </c>
       <c r="K351">
-        <v>48.14814814814815</v>
+        <v>48.15</v>
       </c>
     </row>
     <row r="352">
@@ -13808,7 +13808,7 @@
         <v>27</v>
       </c>
       <c r="K354">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="355">
@@ -13851,7 +13851,7 @@
         <v>27</v>
       </c>
       <c r="K355">
-        <v>3.703703703703703</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="356">
@@ -13894,7 +13894,7 @@
         <v>27</v>
       </c>
       <c r="K356">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="357">
@@ -13968,7 +13968,7 @@
         <v>27</v>
       </c>
       <c r="K358">
-        <v>22.22222222222222</v>
+        <v>22.22</v>
       </c>
     </row>
     <row r="359">
@@ -14008,7 +14008,7 @@
         <v>102</v>
       </c>
       <c r="K359">
-        <v>22.54901960784314</v>
+        <v>22.55</v>
       </c>
     </row>
     <row r="360">
@@ -14144,7 +14144,7 @@
         <v>102</v>
       </c>
       <c r="K363">
-        <v>2.941176470588235</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="364">
@@ -14187,7 +14187,7 @@
         <v>102</v>
       </c>
       <c r="K364">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="365">
@@ -14230,7 +14230,7 @@
         <v>102</v>
       </c>
       <c r="K365">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="366">
@@ -14273,7 +14273,7 @@
         <v>102</v>
       </c>
       <c r="K366">
-        <v>55.88235294117647</v>
+        <v>55.88</v>
       </c>
     </row>
     <row r="367">
@@ -14418,7 +14418,7 @@
         <v>112</v>
       </c>
       <c r="K370">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="371">
@@ -14461,7 +14461,7 @@
         <v>112</v>
       </c>
       <c r="K371">
-        <v>3.571428571428571</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="372">
@@ -14504,7 +14504,7 @@
         <v>112</v>
       </c>
       <c r="K372">
-        <v>1.785714285714286</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="373">
@@ -14547,7 +14547,7 @@
         <v>112</v>
       </c>
       <c r="K373">
-        <v>8.928571428571429</v>
+        <v>8.93</v>
       </c>
     </row>
     <row r="374">
@@ -14590,7 +14590,7 @@
         <v>112</v>
       </c>
       <c r="K374">
-        <v>47.32142857142857</v>
+        <v>47.32</v>
       </c>
     </row>
     <row r="375">
@@ -14630,7 +14630,7 @@
         <v>102</v>
       </c>
       <c r="K375">
-        <v>8.823529411764707</v>
+        <v>8.82</v>
       </c>
     </row>
     <row r="376">
@@ -14673,7 +14673,7 @@
         <v>102</v>
       </c>
       <c r="K376">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="377">
@@ -14747,7 +14747,7 @@
         <v>102</v>
       </c>
       <c r="K378">
-        <v>3.92156862745098</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="379">
@@ -14790,7 +14790,7 @@
         <v>102</v>
       </c>
       <c r="K379">
-        <v>5.88235294117647</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="380">
@@ -14833,7 +14833,7 @@
         <v>102</v>
       </c>
       <c r="K380">
-        <v>3.92156862745098</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="381">
@@ -14876,7 +14876,7 @@
         <v>102</v>
       </c>
       <c r="K381">
-        <v>17.64705882352941</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="382">
@@ -14919,7 +14919,7 @@
         <v>102</v>
       </c>
       <c r="K382">
-        <v>57.84313725490197</v>
+        <v>57.84</v>
       </c>
     </row>
     <row r="383">
@@ -14962,7 +14962,7 @@
         <v>112</v>
       </c>
       <c r="K383">
-        <v>1.785714285714286</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="384">
@@ -15045,7 +15045,7 @@
         <v>112</v>
       </c>
       <c r="K385">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="386">
@@ -15119,7 +15119,7 @@
         <v>112</v>
       </c>
       <c r="K387">
-        <v>1.785714285714286</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="388">
@@ -15162,7 +15162,7 @@
         <v>112</v>
       </c>
       <c r="K388">
-        <v>8.035714285714286</v>
+        <v>8.039999999999999</v>
       </c>
     </row>
     <row r="389">
@@ -15205,7 +15205,7 @@
         <v>112</v>
       </c>
       <c r="K389">
-        <v>3.571428571428571</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="390">
@@ -15248,7 +15248,7 @@
         <v>112</v>
       </c>
       <c r="K390">
-        <v>16.07142857142857</v>
+        <v>16.07</v>
       </c>
     </row>
     <row r="391">
@@ -15291,7 +15291,7 @@
         <v>112</v>
       </c>
       <c r="K391">
-        <v>55.35714285714286</v>
+        <v>55.36</v>
       </c>
     </row>
     <row r="392">
@@ -15334,7 +15334,7 @@
         <v>102</v>
       </c>
       <c r="K392">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="393">
@@ -15448,7 +15448,7 @@
         <v>102</v>
       </c>
       <c r="K395">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="396">
@@ -15491,7 +15491,7 @@
         <v>102</v>
       </c>
       <c r="K396">
-        <v>5.88235294117647</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="397">
@@ -15534,7 +15534,7 @@
         <v>102</v>
       </c>
       <c r="K397">
-        <v>4.901960784313726</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="398">
@@ -15577,7 +15577,7 @@
         <v>102</v>
       </c>
       <c r="K398">
-        <v>5.88235294117647</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="399">
@@ -15620,7 +15620,7 @@
         <v>102</v>
       </c>
       <c r="K399">
-        <v>21.56862745098039</v>
+        <v>21.57</v>
       </c>
     </row>
     <row r="400">
@@ -15663,7 +15663,7 @@
         <v>102</v>
       </c>
       <c r="K400">
-        <v>58.82352941176471</v>
+        <v>58.82</v>
       </c>
     </row>
     <row r="401">
@@ -15706,7 +15706,7 @@
         <v>112</v>
       </c>
       <c r="K401">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="402">
@@ -15820,7 +15820,7 @@
         <v>112</v>
       </c>
       <c r="K404">
-        <v>3.571428571428571</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="405">
@@ -15863,7 +15863,7 @@
         <v>112</v>
       </c>
       <c r="K405">
-        <v>4.464285714285714</v>
+        <v>4.46</v>
       </c>
     </row>
     <row r="406">
@@ -15906,7 +15906,7 @@
         <v>112</v>
       </c>
       <c r="K406">
-        <v>5.357142857142857</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="407">
@@ -15949,7 +15949,7 @@
         <v>112</v>
       </c>
       <c r="K407">
-        <v>9.821428571428571</v>
+        <v>9.82</v>
       </c>
     </row>
     <row r="408">
@@ -15992,7 +15992,7 @@
         <v>112</v>
       </c>
       <c r="K408">
-        <v>11.60714285714286</v>
+        <v>11.61</v>
       </c>
     </row>
     <row r="409">
@@ -16078,7 +16078,7 @@
         <v>102</v>
       </c>
       <c r="K410">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="411">
@@ -16161,7 +16161,7 @@
         <v>102</v>
       </c>
       <c r="K412">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="413">
@@ -16235,7 +16235,7 @@
         <v>102</v>
       </c>
       <c r="K414">
-        <v>3.92156862745098</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="415">
@@ -16278,7 +16278,7 @@
         <v>102</v>
       </c>
       <c r="K415">
-        <v>6.862745098039216</v>
+        <v>6.86</v>
       </c>
     </row>
     <row r="416">
@@ -16321,7 +16321,7 @@
         <v>102</v>
       </c>
       <c r="K416">
-        <v>4.901960784313726</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="417">
@@ -16364,7 +16364,7 @@
         <v>102</v>
       </c>
       <c r="K417">
-        <v>25.49019607843137</v>
+        <v>25.49</v>
       </c>
     </row>
     <row r="418">
@@ -16407,7 +16407,7 @@
         <v>102</v>
       </c>
       <c r="K418">
-        <v>55.88235294117647</v>
+        <v>55.88</v>
       </c>
     </row>
     <row r="419">
@@ -16450,7 +16450,7 @@
         <v>112</v>
       </c>
       <c r="K419">
-        <v>3.571428571428571</v>
+        <v>3.57</v>
       </c>
     </row>
     <row r="420">
@@ -16564,7 +16564,7 @@
         <v>112</v>
       </c>
       <c r="K422">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="423">
@@ -16607,7 +16607,7 @@
         <v>112</v>
       </c>
       <c r="K423">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="424">
@@ -16650,7 +16650,7 @@
         <v>112</v>
       </c>
       <c r="K424">
-        <v>8.035714285714286</v>
+        <v>8.039999999999999</v>
       </c>
     </row>
     <row r="425">
@@ -16693,7 +16693,7 @@
         <v>112</v>
       </c>
       <c r="K425">
-        <v>7.142857142857142</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="426">
@@ -16736,7 +16736,7 @@
         <v>112</v>
       </c>
       <c r="K426">
-        <v>14.28571428571428</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="427">
@@ -16779,7 +16779,7 @@
         <v>112</v>
       </c>
       <c r="K427">
-        <v>61.60714285714286</v>
+        <v>61.61</v>
       </c>
     </row>
     <row r="428">
@@ -16822,7 +16822,7 @@
         <v>102</v>
       </c>
       <c r="K428">
-        <v>5.88235294117647</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="429">
@@ -16967,7 +16967,7 @@
         <v>102</v>
       </c>
       <c r="K432">
-        <v>2.941176470588235</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="433">
@@ -17010,7 +17010,7 @@
         <v>102</v>
       </c>
       <c r="K433">
-        <v>7.84313725490196</v>
+        <v>7.84</v>
       </c>
     </row>
     <row r="434">
@@ -17053,7 +17053,7 @@
         <v>102</v>
       </c>
       <c r="K434">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="435">
@@ -17096,7 +17096,7 @@
         <v>102</v>
       </c>
       <c r="K435">
-        <v>29.41176470588236</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="436">
@@ -17139,7 +17139,7 @@
         <v>102</v>
       </c>
       <c r="K436">
-        <v>51.9607843137255</v>
+        <v>51.96</v>
       </c>
     </row>
     <row r="437">
@@ -17182,7 +17182,7 @@
         <v>112</v>
       </c>
       <c r="K437">
-        <v>7.142857142857142</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="438">
@@ -17296,7 +17296,7 @@
         <v>112</v>
       </c>
       <c r="K440">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="441">
@@ -17339,7 +17339,7 @@
         <v>112</v>
       </c>
       <c r="K441">
-        <v>1.785714285714286</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="442">
@@ -17382,7 +17382,7 @@
         <v>112</v>
       </c>
       <c r="K442">
-        <v>10.71428571428571</v>
+        <v>10.71</v>
       </c>
     </row>
     <row r="443">
@@ -17425,7 +17425,7 @@
         <v>112</v>
       </c>
       <c r="K443">
-        <v>5.357142857142857</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="444">
@@ -17468,7 +17468,7 @@
         <v>112</v>
       </c>
       <c r="K444">
-        <v>13.39285714285714</v>
+        <v>13.39</v>
       </c>
     </row>
     <row r="445">
@@ -17511,7 +17511,7 @@
         <v>112</v>
       </c>
       <c r="K445">
-        <v>58.92857142857143</v>
+        <v>58.93</v>
       </c>
     </row>
     <row r="446">
@@ -17554,7 +17554,7 @@
         <v>102</v>
       </c>
       <c r="K446">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="447">
@@ -17668,7 +17668,7 @@
         <v>102</v>
       </c>
       <c r="K449">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="450">
@@ -17742,7 +17742,7 @@
         <v>102</v>
       </c>
       <c r="K451">
-        <v>2.941176470588235</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="452">
@@ -17816,7 +17816,7 @@
         <v>102</v>
       </c>
       <c r="K453">
-        <v>16.66666666666666</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="454">
@@ -17859,7 +17859,7 @@
         <v>102</v>
       </c>
       <c r="K454">
-        <v>62.74509803921568</v>
+        <v>62.75</v>
       </c>
     </row>
     <row r="455">
@@ -17902,7 +17902,7 @@
         <v>112</v>
       </c>
       <c r="K455">
-        <v>20.53571428571428</v>
+        <v>20.54</v>
       </c>
     </row>
     <row r="456">
@@ -18016,7 +18016,7 @@
         <v>112</v>
       </c>
       <c r="K458">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="459">
@@ -18090,7 +18090,7 @@
         <v>112</v>
       </c>
       <c r="K460">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="461">
@@ -18164,7 +18164,7 @@
         <v>112</v>
       </c>
       <c r="K462">
-        <v>14.28571428571428</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="463">
@@ -18207,7 +18207,7 @@
         <v>112</v>
       </c>
       <c r="K463">
-        <v>61.60714285714286</v>
+        <v>61.61</v>
       </c>
     </row>
     <row r="464">
@@ -18250,7 +18250,7 @@
         <v>102</v>
       </c>
       <c r="K464">
-        <v>37.25490196078432</v>
+        <v>37.25</v>
       </c>
     </row>
     <row r="465">
@@ -18395,7 +18395,7 @@
         <v>102</v>
       </c>
       <c r="K468">
-        <v>2.941176470588235</v>
+        <v>2.94</v>
       </c>
     </row>
     <row r="469">
@@ -18438,7 +18438,7 @@
         <v>102</v>
       </c>
       <c r="K469">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="470">
@@ -18481,7 +18481,7 @@
         <v>102</v>
       </c>
       <c r="K470">
-        <v>17.64705882352941</v>
+        <v>17.65</v>
       </c>
     </row>
     <row r="471">
@@ -18555,7 +18555,7 @@
         <v>102</v>
       </c>
       <c r="K472">
-        <v>41.17647058823529</v>
+        <v>41.18</v>
       </c>
     </row>
     <row r="473">
@@ -18598,7 +18598,7 @@
         <v>112</v>
       </c>
       <c r="K473">
-        <v>21.42857142857143</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="474">
@@ -18743,7 +18743,7 @@
         <v>112</v>
       </c>
       <c r="K477">
-        <v>5.357142857142857</v>
+        <v>5.36</v>
       </c>
     </row>
     <row r="478">
@@ -18786,7 +18786,7 @@
         <v>112</v>
       </c>
       <c r="K478">
-        <v>1.785714285714286</v>
+        <v>1.79</v>
       </c>
     </row>
     <row r="479">
@@ -18829,7 +18829,7 @@
         <v>112</v>
       </c>
       <c r="K479">
-        <v>16.96428571428572</v>
+        <v>16.96</v>
       </c>
     </row>
     <row r="480">
@@ -18903,7 +18903,7 @@
         <v>112</v>
       </c>
       <c r="K481">
-        <v>54.46428571428571</v>
+        <v>54.46</v>
       </c>
     </row>
     <row r="482">
@@ -18946,7 +18946,7 @@
         <v>102</v>
       </c>
       <c r="K482">
-        <v>29.41176470588236</v>
+        <v>29.41</v>
       </c>
     </row>
     <row r="483">
@@ -19091,7 +19091,7 @@
         <v>102</v>
       </c>
       <c r="K486">
-        <v>1.96078431372549</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="487">
@@ -19165,7 +19165,7 @@
         <v>102</v>
       </c>
       <c r="K488">
-        <v>14.70588235294118</v>
+        <v>14.71</v>
       </c>
     </row>
     <row r="489">
@@ -19239,7 +19239,7 @@
         <v>102</v>
       </c>
       <c r="K490">
-        <v>53.92156862745098</v>
+        <v>53.92</v>
       </c>
     </row>
     <row r="491">
@@ -19282,7 +19282,7 @@
         <v>112</v>
       </c>
       <c r="K491">
-        <v>33.03571428571428</v>
+        <v>33.04</v>
       </c>
     </row>
     <row r="492">
@@ -19427,7 +19427,7 @@
         <v>112</v>
       </c>
       <c r="K495">
-        <v>4.464285714285714</v>
+        <v>4.46</v>
       </c>
     </row>
     <row r="496">
@@ -19615,7 +19615,7 @@
         <v>102</v>
       </c>
       <c r="K500">
-        <v>51.9607843137255</v>
+        <v>51.96</v>
       </c>
     </row>
     <row r="501">
@@ -19720,7 +19720,7 @@
         <v>102</v>
       </c>
       <c r="K503">
-        <v>4.901960784313726</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="504">
@@ -19763,7 +19763,7 @@
         <v>102</v>
       </c>
       <c r="K504">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="505">
@@ -19806,7 +19806,7 @@
         <v>102</v>
       </c>
       <c r="K505">
-        <v>11.76470588235294</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="506">
@@ -19880,7 +19880,7 @@
         <v>102</v>
       </c>
       <c r="K507">
-        <v>30.3921568627451</v>
+        <v>30.39</v>
       </c>
     </row>
     <row r="508">
@@ -19923,7 +19923,7 @@
         <v>112</v>
       </c>
       <c r="K508">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="509">
@@ -20068,7 +20068,7 @@
         <v>112</v>
       </c>
       <c r="K512">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="513">
@@ -20111,7 +20111,7 @@
         <v>112</v>
       </c>
       <c r="K513">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="514">
@@ -20154,7 +20154,7 @@
         <v>112</v>
       </c>
       <c r="K514">
-        <v>14.28571428571428</v>
+        <v>14.29</v>
       </c>
     </row>
     <row r="515">
@@ -20271,7 +20271,7 @@
         <v>102</v>
       </c>
       <c r="K517">
-        <v>51.9607843137255</v>
+        <v>51.96</v>
       </c>
     </row>
     <row r="518">
@@ -20416,7 +20416,7 @@
         <v>102</v>
       </c>
       <c r="K521">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="522">
@@ -20459,7 +20459,7 @@
         <v>102</v>
       </c>
       <c r="K522">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="523">
@@ -20502,7 +20502,7 @@
         <v>102</v>
       </c>
       <c r="K523">
-        <v>5.88235294117647</v>
+        <v>5.88</v>
       </c>
     </row>
     <row r="524">
@@ -20576,7 +20576,7 @@
         <v>102</v>
       </c>
       <c r="K525">
-        <v>40.19607843137255</v>
+        <v>40.2</v>
       </c>
     </row>
     <row r="526">
@@ -20616,7 +20616,7 @@
         <v>102</v>
       </c>
       <c r="K526">
-        <v>32.35294117647059</v>
+        <v>32.35</v>
       </c>
     </row>
     <row r="527">
@@ -20721,7 +20721,7 @@
         <v>102</v>
       </c>
       <c r="K529">
-        <v>3.92156862745098</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="530">
@@ -20764,7 +20764,7 @@
         <v>102</v>
       </c>
       <c r="K530">
-        <v>0.9803921568627451</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="531">
@@ -20807,7 +20807,7 @@
         <v>102</v>
       </c>
       <c r="K531">
-        <v>11.76470588235294</v>
+        <v>11.76</v>
       </c>
     </row>
     <row r="532">
@@ -20881,7 +20881,7 @@
         <v>102</v>
       </c>
       <c r="K533">
-        <v>50.98039215686274</v>
+        <v>50.98</v>
       </c>
     </row>
     <row r="534">
@@ -20924,7 +20924,7 @@
         <v>112</v>
       </c>
       <c r="K534">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="535">
@@ -20964,7 +20964,7 @@
         <v>112</v>
       </c>
       <c r="K535">
-        <v>28.57142857142857</v>
+        <v>28.57</v>
       </c>
     </row>
     <row r="536">
@@ -21069,7 +21069,7 @@
         <v>112</v>
       </c>
       <c r="K538">
-        <v>2.678571428571428</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="539">
@@ -21112,7 +21112,7 @@
         <v>112</v>
       </c>
       <c r="K539">
-        <v>0.8928571428571428</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="540">
@@ -21229,7 +21229,7 @@
         <v>112</v>
       </c>
       <c r="K542">
-        <v>60.71428571428571</v>
+        <v>60.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>